<commit_message>
tested all 3 apps
</commit_message>
<xml_diff>
--- a/Office.4dbase/Resources/test.xlsx
+++ b/Office.4dbase/Resources/test.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miyako/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr codeName="ThisWorkbook" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="23040" windowHeight="8840"/>
   </bookViews>
@@ -25,7 +20,7 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -277,9 +272,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="見出し 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="見出し 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1304,7 +1299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Arial">
       <a:majorFont>
-        <a:latin typeface="Arial" panose="020B0604020202020204"/>
+        <a:latin typeface="Arial"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1339,7 +1334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" panose="020B0604020202020204"/>
+        <a:latin typeface="Arial"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1516,7 +1511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1532,7 +1527,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" style="3" customWidth="1"/>
@@ -1541,13 +1536,13 @@
     <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="47" x14ac:dyDescent="0.8">
+    <row r="1" spans="2:3" ht="44">
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:3" ht="37.5" customHeight="1">
       <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
@@ -1555,63 +1550,63 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" ht="30" customHeight="1">
       <c r="B3" s="4"/>
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" ht="20.5" customHeight="1">
       <c r="C4" s="5">
         <f>SUM(Income[金額])</f>
         <v>375000</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" ht="20.5" customHeight="1">
       <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" ht="20.5" customHeight="1">
       <c r="C6" s="5">
         <f>SUM(Expenses[金額])</f>
         <v>205800</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" ht="20.5" customHeight="1">
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="20.5" customHeight="1">
       <c r="C8" s="5">
         <f>SUM(Savings[金額])</f>
         <v>55000</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" ht="20.5" customHeight="1">
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" ht="20.5" customHeight="1">
       <c r="C10" s="5">
         <f>Total_Monthly_Income-Total_Monthly_Expenses-Total_Monthly_Savings</f>
         <v>114200</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" ht="22.5" customHeight="1">
       <c r="B11" s="6">
         <f>MIN(Total_Monthly_Expenses/Total_Monthly_Income,1)</f>
         <v>0.54879999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:3" ht="37.5" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" ht="25" customHeight="1">
       <c r="B13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1619,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" ht="25" customHeight="1">
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1627,7 +1622,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" ht="25" customHeight="1">
       <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1635,7 +1630,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" ht="25" customHeight="1">
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1643,15 +1638,15 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" ht="25" customHeight="1">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:3" ht="25" customHeight="1">
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="25" customHeight="1">
       <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" ht="25" customHeight="1">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1667,7 +1662,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" ht="25" customHeight="1">
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1675,7 +1670,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" ht="25" customHeight="1">
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1678,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" ht="25" customHeight="1">
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
@@ -1691,7 +1686,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" ht="25" customHeight="1">
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1699,7 +1694,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" ht="25" customHeight="1">
       <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
@@ -1707,7 +1702,7 @@
         <v>27300</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" ht="25" customHeight="1">
       <c r="B26" s="3" t="s">
         <v>13</v>
       </c>
@@ -1715,7 +1710,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" ht="25" customHeight="1">
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
@@ -1723,7 +1718,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" ht="25" customHeight="1">
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
@@ -1731,16 +1726,16 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" ht="25" customHeight="1">
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:3" ht="25" customHeight="1">
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" ht="25" customHeight="1">
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
@@ -1748,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" ht="25" customHeight="1">
       <c r="B32" s="10" t="s">
         <v>23</v>
       </c>
@@ -1756,7 +1751,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" ht="25" customHeight="1">
       <c r="B33" s="10" t="s">
         <v>23</v>
       </c>
@@ -1764,7 +1759,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" ht="25" customHeight="1">
       <c r="B34" s="10" t="s">
         <v>23</v>
       </c>
@@ -1776,15 +1771,15 @@
   <phoneticPr fontId="4"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.41" top="0.41" bottom="0.35" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <tableParts count="3">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -1802,6 +1797,9 @@
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -1815,30 +1813,30 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="3" customWidth="1"/>
     <col min="2" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2">
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2">
       <c r="B4" s="11">
         <f>MIN(1-B5,1)</f>
         <v>0.45120000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2">
       <c r="B5" s="11">
         <f>MIN(Total_Monthly_Expenses/Total_Monthly_Income,1)</f>
         <v>0.54879999999999995</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2">
       <c r="B6" s="3" t="b">
         <f>(Total_Monthly_Expenses/Total_Monthly_Income)&gt;1</f>
         <v>0</v>
@@ -1847,6 +1845,11 @@
   </sheetData>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>